<commit_message>
Hardcode dates to get correct data
</commit_message>
<xml_diff>
--- a/populate_data_app/files/generated-energy-usage-by-house-hold-appliances.xlsx
+++ b/populate_data_app/files/generated-energy-usage-by-house-hold-appliances.xlsx
@@ -438,16 +438,16 @@
         <v>4.931506849315069</v>
       </c>
       <c r="H2">
-        <v>143.83561643835617</v>
+        <v>1726.027397260274</v>
       </c>
       <c r="I2" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J2" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K2" t="str">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -476,10 +476,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J3" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K3" t="str">
         <v>0</v>
@@ -511,10 +511,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J4" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K4" t="str">
         <v>0</v>
@@ -546,10 +546,10 @@
         <v>37.442922374429216</v>
       </c>
       <c r="I5" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J5" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K5" t="str">
         <v>2</v>
@@ -581,10 +581,10 @@
         <v>15.410958904109588</v>
       </c>
       <c r="I6" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J6" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K6" t="str">
         <v>1</v>
@@ -613,16 +613,16 @@
         <v>0.4794520547945205</v>
       </c>
       <c r="H7">
-        <v>14.04109589041096</v>
+        <v>42.12328767123288</v>
       </c>
       <c r="I7" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J7" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K7" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -648,16 +648,16 @@
         <v>0.4273972602739726</v>
       </c>
       <c r="H8">
-        <v>49.77168949771689</v>
+        <v>37.32876712328767</v>
       </c>
       <c r="I8" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J8" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K8" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -683,16 +683,16 @@
         <v>0.2356164383561644</v>
       </c>
       <c r="H9">
-        <v>3.424657534246575</v>
+        <v>6.84931506849315</v>
       </c>
       <c r="I9" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J9" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K9" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -718,16 +718,16 @@
         <v>0.19726027397260273</v>
       </c>
       <c r="H10">
-        <v>0.5707762557077626</v>
+        <v>5.707762557077626</v>
       </c>
       <c r="I10" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J10" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K10" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -753,16 +753,16 @@
         <v>0.1863013698630137</v>
       </c>
       <c r="H11">
-        <v>0.547945205479452</v>
+        <v>5.479452054794519</v>
       </c>
       <c r="I11" t="str">
-        <v>6/3/2022</v>
+        <v>28/11/2021</v>
       </c>
       <c r="J11" t="str">
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="K11" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -788,16 +788,16 @@
         <v>4.931506849315069</v>
       </c>
       <c r="H12">
-        <v>143.83561643835617</v>
+        <v>1869.86301369863</v>
       </c>
       <c r="I12" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J12" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K12" t="str">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -826,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J13" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K13" t="str">
         <v>0</v>
@@ -861,10 +861,10 @@
         <v>0</v>
       </c>
       <c r="I14" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J14" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K14" t="str">
         <v>0</v>
@@ -893,16 +893,16 @@
         <v>0.6410958904109589</v>
       </c>
       <c r="H15">
-        <v>37.442922374429216</v>
+        <v>56.16438356164383</v>
       </c>
       <c r="I15" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J15" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K15" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -931,10 +931,10 @@
         <v>15.410958904109588</v>
       </c>
       <c r="I16" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J16" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K16" t="str">
         <v>1</v>
@@ -963,16 +963,16 @@
         <v>0.4794520547945205</v>
       </c>
       <c r="H17">
-        <v>14.04109589041096</v>
+        <v>56.16438356164384</v>
       </c>
       <c r="I17" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J17" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K17" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1001,10 +1001,10 @@
         <v>49.77168949771689</v>
       </c>
       <c r="I18" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J18" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K18" t="str">
         <v>4</v>
@@ -1033,16 +1033,16 @@
         <v>0.2356164383561644</v>
       </c>
       <c r="H19">
-        <v>3.424657534246575</v>
+        <v>6.84931506849315</v>
       </c>
       <c r="I19" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J19" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K19" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1068,16 +1068,16 @@
         <v>0.19726027397260273</v>
       </c>
       <c r="H20">
-        <v>0.5707762557077626</v>
+        <v>5.707762557077626</v>
       </c>
       <c r="I20" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J20" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K20" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1103,16 +1103,16 @@
         <v>0.1863013698630137</v>
       </c>
       <c r="H21">
-        <v>0.547945205479452</v>
+        <v>5.479452054794519</v>
       </c>
       <c r="I21" t="str">
-        <v>6/3/2022</v>
+        <v>29/11/2021</v>
       </c>
       <c r="J21" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="K21" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1138,16 +1138,16 @@
         <v>4.931506849315069</v>
       </c>
       <c r="H22">
-        <v>143.83561643835617</v>
+        <v>1869.86301369863</v>
       </c>
       <c r="I22" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J22" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K22" t="str">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -1176,10 +1176,10 @@
         <v>0</v>
       </c>
       <c r="I23" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J23" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K23" t="str">
         <v>0</v>
@@ -1211,10 +1211,10 @@
         <v>0</v>
       </c>
       <c r="I24" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J24" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K24" t="str">
         <v>0</v>
@@ -1243,16 +1243,16 @@
         <v>0.6410958904109589</v>
       </c>
       <c r="H25">
-        <v>37.442922374429216</v>
+        <v>18.721461187214608</v>
       </c>
       <c r="I25" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J25" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K25" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1281,10 +1281,10 @@
         <v>15.410958904109588</v>
       </c>
       <c r="I26" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J26" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K26" t="str">
         <v>1</v>
@@ -1313,16 +1313,16 @@
         <v>0.4794520547945205</v>
       </c>
       <c r="H27">
-        <v>14.04109589041096</v>
+        <v>28.08219178082192</v>
       </c>
       <c r="I27" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J27" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K27" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1348,16 +1348,16 @@
         <v>0.4273972602739726</v>
       </c>
       <c r="H28">
-        <v>49.77168949771689</v>
+        <v>24.885844748858446</v>
       </c>
       <c r="I28" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J28" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K28" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1383,16 +1383,16 @@
         <v>0.2356164383561644</v>
       </c>
       <c r="H29">
-        <v>3.424657534246575</v>
+        <v>0</v>
       </c>
       <c r="I29" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J29" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K29" t="str">
-        <v>0.5</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -1418,16 +1418,16 @@
         <v>0.19726027397260273</v>
       </c>
       <c r="H30">
-        <v>0.5707762557077626</v>
+        <v>5.707762557077626</v>
       </c>
       <c r="I30" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J30" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K30" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1453,16 +1453,16 @@
         <v>0.1863013698630137</v>
       </c>
       <c r="H31">
-        <v>0.547945205479452</v>
+        <v>5.479452054794519</v>
       </c>
       <c r="I31" t="str">
-        <v>6/3/2022</v>
+        <v>1/12/2021</v>
       </c>
       <c r="J31" t="str">
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="K31" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1488,16 +1488,16 @@
         <v>4.931506849315069</v>
       </c>
       <c r="H32">
-        <v>143.83561643835617</v>
+        <v>1438.3561643835617</v>
       </c>
       <c r="I32" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J32" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K32" t="str">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33">
@@ -1526,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="I33" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J33" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K33" t="str">
         <v>0</v>
@@ -1561,10 +1561,10 @@
         <v>0</v>
       </c>
       <c r="I34" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J34" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K34" t="str">
         <v>0</v>
@@ -1596,10 +1596,10 @@
         <v>37.442922374429216</v>
       </c>
       <c r="I35" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J35" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K35" t="str">
         <v>2</v>
@@ -1631,10 +1631,10 @@
         <v>15.410958904109588</v>
       </c>
       <c r="I36" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J36" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K36" t="str">
         <v>1</v>
@@ -1663,16 +1663,16 @@
         <v>0.4794520547945205</v>
       </c>
       <c r="H37">
-        <v>14.04109589041096</v>
+        <v>28.08219178082192</v>
       </c>
       <c r="I37" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J37" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K37" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1698,16 +1698,16 @@
         <v>0.4273972602739726</v>
       </c>
       <c r="H38">
-        <v>49.77168949771689</v>
+        <v>24.885844748858446</v>
       </c>
       <c r="I38" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J38" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K38" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1733,16 +1733,16 @@
         <v>0.2356164383561644</v>
       </c>
       <c r="H39">
-        <v>3.424657534246575</v>
+        <v>13.6986301369863</v>
       </c>
       <c r="I39" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J39" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K39" t="str">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1768,16 +1768,16 @@
         <v>0.19726027397260273</v>
       </c>
       <c r="H40">
-        <v>0.5707762557077626</v>
+        <v>5.707762557077626</v>
       </c>
       <c r="I40" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J40" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K40" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1803,16 +1803,16 @@
         <v>0.1863013698630137</v>
       </c>
       <c r="H41">
-        <v>0.547945205479452</v>
+        <v>5.479452054794519</v>
       </c>
       <c r="I41" t="str">
-        <v>6/3/2022</v>
+        <v>2/12/2021</v>
       </c>
       <c r="J41" t="str">
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="K41" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1838,16 +1838,16 @@
         <v>4.931506849315069</v>
       </c>
       <c r="H42">
-        <v>143.83561643835617</v>
+        <v>1869.86301369863</v>
       </c>
       <c r="I42" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J42" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K42" t="str">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43">
@@ -1876,10 +1876,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J43" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K43" t="str">
         <v>0</v>
@@ -1911,10 +1911,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J44" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K44" t="str">
         <v>0</v>
@@ -1943,16 +1943,16 @@
         <v>0.6410958904109589</v>
       </c>
       <c r="H45">
-        <v>37.442922374429216</v>
+        <v>18.721461187214608</v>
       </c>
       <c r="I45" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J45" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K45" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1981,10 +1981,10 @@
         <v>15.410958904109588</v>
       </c>
       <c r="I46" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J46" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K46" t="str">
         <v>1</v>
@@ -2013,16 +2013,16 @@
         <v>0.4794520547945205</v>
       </c>
       <c r="H47">
-        <v>14.04109589041096</v>
+        <v>42.12328767123288</v>
       </c>
       <c r="I47" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J47" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K47" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -2048,16 +2048,16 @@
         <v>0.4273972602739726</v>
       </c>
       <c r="H48">
-        <v>49.77168949771689</v>
+        <v>37.32876712328767</v>
       </c>
       <c r="I48" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J48" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K48" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -2083,16 +2083,16 @@
         <v>0.2356164383561644</v>
       </c>
       <c r="H49">
-        <v>3.424657534246575</v>
+        <v>6.84931506849315</v>
       </c>
       <c r="I49" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J49" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K49" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2118,16 +2118,16 @@
         <v>0.19726027397260273</v>
       </c>
       <c r="H50">
-        <v>0.5707762557077626</v>
+        <v>5.707762557077626</v>
       </c>
       <c r="I50" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J50" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K50" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -2153,16 +2153,16 @@
         <v>0.1863013698630137</v>
       </c>
       <c r="H51">
-        <v>0.547945205479452</v>
+        <v>5.479452054794519</v>
       </c>
       <c r="I51" t="str">
-        <v>6/3/2022</v>
+        <v>3/12/2021</v>
       </c>
       <c r="J51" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="K51" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2188,16 +2188,16 @@
         <v>4.931506849315069</v>
       </c>
       <c r="H52">
-        <v>143.83561643835617</v>
+        <v>1438.3561643835617</v>
       </c>
       <c r="I52" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J52" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K52" t="str">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53">
@@ -2226,10 +2226,10 @@
         <v>0</v>
       </c>
       <c r="I53" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J53" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K53" t="str">
         <v>0</v>
@@ -2261,10 +2261,10 @@
         <v>0</v>
       </c>
       <c r="I54" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J54" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K54" t="str">
         <v>0</v>
@@ -2296,10 +2296,10 @@
         <v>37.442922374429216</v>
       </c>
       <c r="I55" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J55" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K55" t="str">
         <v>2</v>
@@ -2331,10 +2331,10 @@
         <v>15.410958904109588</v>
       </c>
       <c r="I56" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J56" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K56" t="str">
         <v>1</v>
@@ -2363,16 +2363,16 @@
         <v>0.4794520547945205</v>
       </c>
       <c r="H57">
-        <v>14.04109589041096</v>
+        <v>28.08219178082192</v>
       </c>
       <c r="I57" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J57" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K57" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -2398,16 +2398,16 @@
         <v>0.4273972602739726</v>
       </c>
       <c r="H58">
-        <v>49.77168949771689</v>
+        <v>24.885844748858446</v>
       </c>
       <c r="I58" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J58" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K58" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -2433,16 +2433,16 @@
         <v>0.2356164383561644</v>
       </c>
       <c r="H59">
-        <v>3.424657534246575</v>
+        <v>6.84931506849315</v>
       </c>
       <c r="I59" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J59" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K59" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2468,16 +2468,16 @@
         <v>0.19726027397260273</v>
       </c>
       <c r="H60">
-        <v>0.5707762557077626</v>
+        <v>5.707762557077626</v>
       </c>
       <c r="I60" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J60" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K60" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2503,16 +2503,16 @@
         <v>0.1863013698630137</v>
       </c>
       <c r="H61">
-        <v>0.547945205479452</v>
+        <v>5.479452054794519</v>
       </c>
       <c r="I61" t="str">
-        <v>6/3/2022</v>
+        <v>4/12/2021</v>
       </c>
       <c r="J61" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="K61" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2538,16 +2538,16 @@
         <v>4.931506849315069</v>
       </c>
       <c r="H62">
-        <v>143.83561643835617</v>
+        <v>1869.86301369863</v>
       </c>
       <c r="I62" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J62" t="str">
         <v>Saturday</v>
       </c>
       <c r="K62" t="str">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63">
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="I63" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J63" t="str">
         <v>Saturday</v>
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J64" t="str">
         <v>Saturday</v>
@@ -2643,16 +2643,16 @@
         <v>0.6410958904109589</v>
       </c>
       <c r="H65">
-        <v>37.442922374429216</v>
+        <v>18.721461187214608</v>
       </c>
       <c r="I65" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J65" t="str">
         <v>Saturday</v>
       </c>
       <c r="K65" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2681,7 +2681,7 @@
         <v>15.410958904109588</v>
       </c>
       <c r="I66" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J66" t="str">
         <v>Saturday</v>
@@ -2713,16 +2713,16 @@
         <v>0.4794520547945205</v>
       </c>
       <c r="H67">
-        <v>14.04109589041096</v>
+        <v>56.16438356164384</v>
       </c>
       <c r="I67" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J67" t="str">
         <v>Saturday</v>
       </c>
       <c r="K67" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68">
@@ -2751,7 +2751,7 @@
         <v>49.77168949771689</v>
       </c>
       <c r="I68" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J68" t="str">
         <v>Saturday</v>
@@ -2783,16 +2783,16 @@
         <v>0.2356164383561644</v>
       </c>
       <c r="H69">
-        <v>3.424657534246575</v>
+        <v>6.84931506849315</v>
       </c>
       <c r="I69" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J69" t="str">
         <v>Saturday</v>
       </c>
       <c r="K69" t="str">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2818,16 +2818,16 @@
         <v>0.19726027397260273</v>
       </c>
       <c r="H70">
-        <v>0.5707762557077626</v>
+        <v>5.707762557077626</v>
       </c>
       <c r="I70" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J70" t="str">
         <v>Saturday</v>
       </c>
       <c r="K70" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2853,16 +2853,16 @@
         <v>0.1863013698630137</v>
       </c>
       <c r="H71">
-        <v>0.547945205479452</v>
+        <v>5.479452054794519</v>
       </c>
       <c r="I71" t="str">
-        <v>6/3/2022</v>
+        <v>5/12/2021</v>
       </c>
       <c r="J71" t="str">
         <v>Saturday</v>
       </c>
       <c r="K71" t="str">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>